<commit_message>
resimler yerlestirildi yazilar yenilenecek
</commit_message>
<xml_diff>
--- a/overallBurden.xlsx
+++ b/overallBurden.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="24855" windowHeight="12015"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21080"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,7 +65,17 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="tr-TR"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -69,15 +84,16 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11147589803902803"/>
-          <c:y val="3.7763662284090664E-2"/>
-          <c:w val="0.86653509992482503"/>
-          <c:h val="0.84284004423374448"/>
+          <c:x val="0.111475898039028"/>
+          <c:y val="0.0377636622840907"/>
+          <c:w val="0.866535099924825"/>
+          <c:h val="0.842840044233745"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -88,12 +104,13 @@
               </a:schemeClr>
             </a:solidFill>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numLit>
               <c:formatCode>General</c:formatCode>
               <c:ptCount val="1"/>
               <c:pt idx="0">
-                <c:v>95899</c:v>
+                <c:v>160858.0</c:v>
               </c:pt>
             </c:numLit>
           </c:val>
@@ -106,12 +123,13 @@
               <a:schemeClr val="tx1"/>
             </a:solidFill>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numLit>
               <c:formatCode>General</c:formatCode>
               <c:ptCount val="1"/>
               <c:pt idx="0">
-                <c:v>2078</c:v>
+                <c:v>2660.0</c:v>
               </c:pt>
             </c:numLit>
           </c:val>
@@ -119,12 +137,13 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numLit>
               <c:formatCode>General</c:formatCode>
               <c:ptCount val="1"/>
               <c:pt idx="0">
-                <c:v>1</c:v>
+                <c:v>1.0</c:v>
               </c:pt>
             </c:numLit>
           </c:val>
@@ -139,12 +158,13 @@
               </a:schemeClr>
             </a:solidFill>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numLit>
               <c:formatCode>General</c:formatCode>
               <c:ptCount val="1"/>
               <c:pt idx="0">
-                <c:v>101681</c:v>
+                <c:v>168296.0</c:v>
               </c:pt>
             </c:numLit>
           </c:val>
@@ -157,12 +177,13 @@
               <a:prstClr val="black"/>
             </a:solidFill>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numLit>
               <c:formatCode>General</c:formatCode>
               <c:ptCount val="1"/>
               <c:pt idx="0">
-                <c:v>1756</c:v>
+                <c:v>2062.0</c:v>
               </c:pt>
             </c:numLit>
           </c:val>
@@ -170,12 +191,13 @@
         <c:ser>
           <c:idx val="5"/>
           <c:order val="5"/>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numLit>
               <c:formatCode>General</c:formatCode>
               <c:ptCount val="1"/>
               <c:pt idx="0">
-                <c:v>1</c:v>
+                <c:v>1.0</c:v>
               </c:pt>
             </c:numLit>
           </c:val>
@@ -190,12 +212,13 @@
               </a:prstClr>
             </a:solidFill>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numLit>
               <c:formatCode>General</c:formatCode>
               <c:ptCount val="1"/>
               <c:pt idx="0">
-                <c:v>105335</c:v>
+                <c:v>176792.0</c:v>
               </c:pt>
             </c:numLit>
           </c:val>
@@ -208,56 +231,71 @@
               <a:prstClr val="black"/>
             </a:solidFill>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numLit>
               <c:formatCode>General</c:formatCode>
               <c:ptCount val="1"/>
               <c:pt idx="0">
-                <c:v>1832</c:v>
+                <c:v>2558.0</c:v>
               </c:pt>
             </c:numLit>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="38260736"/>
-        <c:axId val="38262272"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2085316408"/>
+        <c:axId val="2085281320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="38260736"/>
+        <c:axId val="2085316408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="38262272"/>
+        <c:crossAx val="2085281320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="38262272"/>
+        <c:axId val="2085281320"/>
         <c:scaling>
-          <c:logBase val="10"/>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="38260736"/>
+        <c:crossAx val="2085316408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -266,7 +304,17 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="tr-TR"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -275,15 +323,16 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.11147589803902799"/>
-          <c:y val="3.7763662284090678E-2"/>
-          <c:w val="0.86653509992482503"/>
-          <c:h val="0.84284004423374481"/>
+          <c:x val="0.111475898039028"/>
+          <c:y val="0.0377636622840907"/>
+          <c:w val="0.866535099924825"/>
+          <c:h val="0.842840044233745"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -294,12 +343,13 @@
               </a:schemeClr>
             </a:solidFill>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numLit>
               <c:formatCode>General</c:formatCode>
               <c:ptCount val="1"/>
               <c:pt idx="0">
-                <c:v>958</c:v>
+                <c:v>963.0</c:v>
               </c:pt>
             </c:numLit>
           </c:val>
@@ -312,12 +362,13 @@
               <a:schemeClr val="tx1"/>
             </a:solidFill>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numLit>
               <c:formatCode>General</c:formatCode>
               <c:ptCount val="1"/>
               <c:pt idx="0">
-                <c:v>20</c:v>
+                <c:v>15.0</c:v>
               </c:pt>
             </c:numLit>
           </c:val>
@@ -325,12 +376,13 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numLit>
               <c:formatCode>General</c:formatCode>
               <c:ptCount val="1"/>
               <c:pt idx="0">
-                <c:v>1</c:v>
+                <c:v>1.0</c:v>
               </c:pt>
             </c:numLit>
           </c:val>
@@ -345,12 +397,13 @@
               </a:schemeClr>
             </a:solidFill>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numLit>
               <c:formatCode>General</c:formatCode>
               <c:ptCount val="1"/>
               <c:pt idx="0">
-                <c:v>1016</c:v>
+                <c:v>1013.0</c:v>
               </c:pt>
             </c:numLit>
           </c:val>
@@ -363,12 +416,13 @@
               <a:prstClr val="black"/>
             </a:solidFill>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numLit>
               <c:formatCode>General</c:formatCode>
               <c:ptCount val="1"/>
               <c:pt idx="0">
-                <c:v>17</c:v>
+                <c:v>12.0</c:v>
               </c:pt>
             </c:numLit>
           </c:val>
@@ -376,12 +430,13 @@
         <c:ser>
           <c:idx val="5"/>
           <c:order val="5"/>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numLit>
               <c:formatCode>General</c:formatCode>
               <c:ptCount val="1"/>
               <c:pt idx="0">
-                <c:v>1</c:v>
+                <c:v>1.0</c:v>
               </c:pt>
             </c:numLit>
           </c:val>
@@ -396,12 +451,13 @@
               </a:prstClr>
             </a:solidFill>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numLit>
               <c:formatCode>General</c:formatCode>
               <c:ptCount val="1"/>
               <c:pt idx="0">
-                <c:v>1053</c:v>
+                <c:v>1058.0</c:v>
               </c:pt>
             </c:numLit>
           </c:val>
@@ -414,55 +470,71 @@
               <a:prstClr val="black"/>
             </a:solidFill>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numLit>
               <c:formatCode>General</c:formatCode>
               <c:ptCount val="1"/>
               <c:pt idx="0">
-                <c:v>18</c:v>
+                <c:v>15.0</c:v>
               </c:pt>
             </c:numLit>
           </c:val>
         </c:ser>
-        <c:axId val="70969984"/>
-        <c:axId val="73949568"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2086439288"/>
+        <c:axId val="2086442136"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="70969984"/>
+        <c:axId val="2086439288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="73949568"/>
+        <c:crossAx val="2086442136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73949568"/>
+        <c:axId val="2086442136"/>
         <c:scaling>
-          <c:logBase val="10"/>
+          <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70969984"/>
+        <c:crossAx val="2086439288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -1632,40 +1704,55 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F24" workbookViewId="0">
-      <selection activeCell="K60" sqref="K60"/>
+    <sheetView tabSelected="1" topLeftCell="F9" workbookViewId="0">
+      <selection activeCell="S25" sqref="S25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>